<commit_message>
2020.06.02 - First commit of full code reconstruction
- added variables.h to handle variables definitions and remove them from definitions.h
- definitions.h is dedicated to definitions only (#define and others)
- starting adding comments to create documentation automatically using DoxyGen
- added DoxyGen output folder with a first test in it.
</commit_message>
<xml_diff>
--- a/LCD_20x4_string_check_and_chr_generator.xlsx
+++ b/LCD_20x4_string_check_and_chr_generator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paride/Workarea/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paride/Workarea/Arduino/ArduTempMonitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0DDED6C-2D5A-4844-8817-42CC566951C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE66CFEA-B635-994F-BDD1-D67C6531E40C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23160" yWindow="1960" windowWidth="28040" windowHeight="17440" xr2:uid="{E79167E5-5269-0C4F-9F81-B943B89F36F0}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
   <si>
     <t>o</t>
   </si>
@@ -170,6 +169,27 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -722,7 +742,7 @@
   <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1196,6 +1216,60 @@
       </c>
     </row>
     <row r="7" spans="1:34" s="5" customFormat="1" ht="26" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="U7" s="4"/>
       <c r="W7" s="9" t="s">
         <v>9</v>

</xml_diff>